<commit_message>
revised binary data to include high and low grazed
</commit_message>
<xml_diff>
--- a/prelimresults.xlsx
+++ b/prelimresults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\PostDoc\grazing.meta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF382655-D7F4-47C3-9579-DD85697927FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD897DD-05B2-452B-94E2-ACCBB05E6096}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="1" xr2:uid="{29A67784-EA28-423E-91C7-BC74C435524A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{29A67784-EA28-423E-91C7-BC74C435524A}"/>
   </bookViews>
   <sheets>
     <sheet name="main.model" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
   <si>
     <t>estimate</t>
   </si>
@@ -48,9 +48,6 @@
     <t>***</t>
   </si>
   <si>
-    <t>higher.taxaInvertebrate</t>
-  </si>
-  <si>
     <t>**</t>
   </si>
   <si>
@@ -60,12 +57,6 @@
     <t>Diversity</t>
   </si>
   <si>
-    <t>Fitness</t>
-  </si>
-  <si>
-    <t>higher.taxaMicrobial</t>
-  </si>
-  <si>
     <t>All</t>
   </si>
   <si>
@@ -121,6 +112,12 @@
   </si>
   <si>
     <t>indigenous</t>
+  </si>
+  <si>
+    <t>Invertebrate</t>
+  </si>
+  <si>
+    <t>Microbial</t>
   </si>
 </sst>
 </file>
@@ -162,14 +159,85 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="39">
+  <dxfs count="46">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -870,10 +938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF5DC862-EE41-4D01-9E32-5A406097DF5C}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,20 +949,17 @@
     <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -908,51 +973,39 @@
       <c r="F2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>0.44469999999999998</v>
+        <v>0.53</v>
       </c>
       <c r="C3">
-        <v>8.9200000000000002E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3">
-        <v>0.73640000000000005</v>
+        <v>0.82889999999999997</v>
       </c>
       <c r="F3">
-        <v>2.47E-2</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="G3" t="s">
         <v>3</v>
       </c>
-      <c r="H3">
-        <v>-0.98780000000000001</v>
-      </c>
-      <c r="I3">
-        <v>0.45340000000000003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>2.8730000000000002</v>
+        <v>2.87</v>
       </c>
       <c r="C4">
-        <v>1.35E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
@@ -961,41 +1014,38 @@
         <v>0.37340000000000001</v>
       </c>
       <c r="F4">
-        <v>0.76270000000000004</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5">
-        <v>0.2099</v>
-      </c>
-      <c r="C5">
-        <v>0.2336</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1.0664</v>
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="C5" s="1">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.07</v>
       </c>
       <c r="F5" s="1">
-        <v>7.4200000000000002E-2</v>
+        <v>3.9E-2</v>
       </c>
       <c r="G5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>-3.9800000000000002E-2</v>
-      </c>
-      <c r="I5">
-        <v>0.96960000000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6">
-        <v>3.3380999999999998</v>
+        <v>3.34</v>
       </c>
       <c r="C6">
         <v>2.0000000000000001E-4</v>
@@ -1004,106 +1054,88 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>0.38</v>
+      </c>
+      <c r="C7">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>-0.54</v>
+      </c>
+      <c r="C8">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>0.67</v>
+      </c>
+      <c r="C9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E9">
+        <v>1.28</v>
+      </c>
+      <c r="F9">
+        <v>7.3000000000000001E-3</v>
+      </c>
+      <c r="G9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B7">
-        <v>0.38429999999999997</v>
-      </c>
-      <c r="C7">
-        <v>0.1943</v>
-      </c>
-      <c r="H7">
-        <v>0.61529999999999996</v>
-      </c>
-      <c r="I7">
-        <v>0.38400000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8">
-        <v>-0.50580000000000003</v>
-      </c>
-      <c r="C8">
-        <v>0.44059999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0.85609999999999997</v>
-      </c>
-      <c r="C9" s="1">
-        <v>5.11E-2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9">
-        <v>1.6756</v>
-      </c>
-      <c r="F9">
-        <v>1.6999999999999999E-3</v>
-      </c>
-      <c r="G9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
       <c r="B10">
-        <v>0.25600000000000001</v>
+        <v>0.41</v>
       </c>
       <c r="C10">
-        <v>0.3145</v>
+        <v>0.13</v>
       </c>
       <c r="E10">
-        <v>0.46829999999999999</v>
+        <v>0.42</v>
       </c>
       <c r="F10">
-        <v>0.61839999999999995</v>
-      </c>
-      <c r="H10">
-        <v>1.5468999999999999</v>
-      </c>
-      <c r="I10">
-        <v>2.06E-2</v>
-      </c>
-      <c r="J10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B11">
-        <v>-0.19020000000000001</v>
+        <v>-0.19</v>
       </c>
       <c r="C11">
-        <v>0.45590000000000003</v>
+        <v>0.46</v>
       </c>
       <c r="E11" s="1">
-        <v>-0.89159999999999995</v>
+        <v>-0.79159999999999997</v>
       </c>
       <c r="F11" s="1">
-        <v>7.0900000000000005E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="G11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
@@ -1112,192 +1144,207 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B14">
-        <v>1.0394000000000001</v>
+        <v>0.99</v>
       </c>
       <c r="C14">
         <v>2.3999999999999998E-3</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E14">
-        <v>0.3886</v>
+        <v>0.39</v>
       </c>
       <c r="F14">
-        <v>0.49780000000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B15">
-        <v>1.3466</v>
+        <v>1.25</v>
       </c>
       <c r="C15">
-        <v>6.8999999999999999E-3</v>
+        <v>8.6999999999999994E-3</v>
       </c>
       <c r="D15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B16">
-        <v>0.36259999999999998</v>
+        <v>0.37</v>
       </c>
       <c r="C16">
-        <v>0.20519999999999999</v>
+        <v>0.17</v>
       </c>
       <c r="E16">
-        <v>0.73099999999999998</v>
+        <v>0.88</v>
       </c>
       <c r="F16">
-        <v>0.50260000000000005</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B17">
-        <v>0.2223</v>
+        <v>0.77</v>
       </c>
       <c r="C17">
-        <v>0.70520000000000005</v>
+        <v>0.25</v>
       </c>
       <c r="E17">
-        <v>0.50439999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="F17">
-        <v>0.56330000000000002</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B18">
-        <v>0.71179999999999999</v>
+        <v>0.71</v>
       </c>
       <c r="C18">
-        <v>0.32950000000000002</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="1">
-        <v>0.91159999999999997</v>
-      </c>
-      <c r="C19" s="1">
-        <v>9.0700000000000003E-2</v>
-      </c>
-      <c r="D19" t="s">
-        <v>2</v>
+        <v>13</v>
+      </c>
+      <c r="B19">
+        <v>0.82</v>
+      </c>
+      <c r="C19">
+        <v>0.11</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B20">
-        <v>1.5526</v>
+        <v>1.19</v>
       </c>
       <c r="C20">
-        <v>4.0800000000000003E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D20" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E20">
-        <v>1.5503</v>
+        <v>0.87</v>
       </c>
       <c r="F20">
-        <v>0.1734</v>
+        <v>1.1100000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21">
+        <v>-0.85</v>
+      </c>
+      <c r="C21">
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="D21" t="s">
         <v>5</v>
       </c>
-      <c r="B21">
-        <v>-0.94379999999999997</v>
-      </c>
-      <c r="C21">
-        <v>6.4000000000000003E-3</v>
-      </c>
-      <c r="D21" t="s">
-        <v>6</v>
-      </c>
       <c r="E21">
-        <v>-0.78090000000000004</v>
+        <v>-0.79</v>
       </c>
       <c r="F21">
-        <v>0.27929999999999999</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B22">
-        <v>-0.98560000000000003</v>
+        <v>-0.89</v>
       </c>
       <c r="C22">
-        <v>0.1095</v>
+        <v>0.13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C3:C11 C14:C22">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="lessThan">
+  <conditionalFormatting sqref="C3:C4 C14:C18 C6:C11 C20:C22">
+    <cfRule type="cellIs" dxfId="23" priority="15" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B11 B14:B20 B22">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
+  <conditionalFormatting sqref="B4 B14:B18 B22 B6:B11 B8:C9 B20">
+    <cfRule type="cellIs" dxfId="22" priority="14" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="13" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F5 F20:F21 F16:F17 F14 F9:F11">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="12" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H10:J10">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
-      <formula>0.05</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="9" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="7" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="greaterThan">
       <formula>1.6756</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="greaterThan">
+      <formula>0.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:C5">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>0.98</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19:C19">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1308,7 +1355,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2CD3222-0374-4489-AFEA-89A8BA041492}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1319,24 +1366,24 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1353,7 +1400,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1370,7 +1417,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1387,24 +1434,24 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
         <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1421,7 +1468,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C8">
         <v>0</v>

</xml_diff>

<commit_message>
created a script to check through the data and begun separating the invertebrates from vertebrates
</commit_message>
<xml_diff>
--- a/prelimresults.xlsx
+++ b/prelimresults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\PostDoc\grazing.meta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD897DD-05B2-452B-94E2-ACCBB05E6096}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A642E1-046D-4098-AE4B-FBF39D07E36E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{29A67784-EA28-423E-91C7-BC74C435524A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945" xr2:uid="{29A67784-EA28-423E-91C7-BC74C435524A}"/>
   </bookViews>
   <sheets>
     <sheet name="main.model" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
   <si>
     <t>estimate</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Diversity</t>
   </si>
   <si>
-    <t>All</t>
-  </si>
-  <si>
     <t>Detrivorous</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
     <t>diversity</t>
   </si>
   <si>
-    <t>fitness</t>
-  </si>
-  <si>
     <t>year</t>
   </si>
   <si>
@@ -118,6 +112,9 @@
   </si>
   <si>
     <t>Microbial</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -167,337 +164,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="46">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="13">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -940,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF5DC862-EE41-4D01-9E32-5A406097DF5C}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,7 +626,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -976,7 +643,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>0.53</v>
@@ -999,7 +666,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>2.87</v>
@@ -1019,7 +686,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1">
         <v>0.32</v>
@@ -1042,7 +709,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>3.34</v>
@@ -1056,7 +723,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>0.38</v>
@@ -1067,7 +734,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>-0.54</v>
@@ -1078,7 +745,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>0.67</v>
@@ -1098,7 +765,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>0.41</v>
@@ -1115,7 +782,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B11">
         <v>-0.19</v>
@@ -1135,7 +802,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
@@ -1146,7 +813,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B14">
         <v>0.99</v>
@@ -1166,7 +833,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15">
         <v>1.25</v>
@@ -1180,7 +847,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16">
         <v>0.37</v>
@@ -1197,7 +864,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17">
         <v>0.77</v>
@@ -1214,7 +881,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18">
         <v>0.71</v>
@@ -1225,7 +892,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19">
         <v>0.82</v>
@@ -1236,7 +903,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20">
         <v>1.19</v>
@@ -1256,7 +923,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B21">
         <v>-0.85</v>
@@ -1276,7 +943,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B22">
         <v>-0.89</v>
@@ -1287,53 +954,53 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3:C4 C14:C18 C6:C11 C20:C22">
-    <cfRule type="cellIs" dxfId="23" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4 B14:B18 B22 B6:B11 B8:C9 B20">
-    <cfRule type="cellIs" dxfId="22" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="14" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="cellIs" dxfId="21" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="13" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F5 F20:F21 F16:F17 F14 F9:F11">
-    <cfRule type="cellIs" dxfId="20" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="18" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThan">
       <formula>1.6756</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1353,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2CD3222-0374-4489-AFEA-89A8BA041492}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1366,24 +1033,24 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>23</v>
-      </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1400,58 +1067,58 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="D5" t="s">
         <v>21</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="F6" t="s">
-        <v>25</v>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1463,23 +1130,6 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
         <v>0</v>
       </c>
     </row>

</xml_diff>